<commit_message>
fix: have correct types for searchCheckBoxOptions and fix typos in the raw dataset
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -3047,13 +3047,13 @@
     <t>2-patch</t>
   </si>
   <si>
-    <t>Continuous Space (1D or 2D))</t>
-  </si>
-  <si>
-    <t>Metapopulation (Finite or Infinite))</t>
-  </si>
-  <si>
-    <t>Stepping Stone (1D, 2D)</t>
+    <t>Continuous Space (1D or 2D)</t>
+  </si>
+  <si>
+    <t>Metapopulation (Finite or Infinite)</t>
+  </si>
+  <si>
+    <t>Stepping Stone (1D or 2D)</t>
   </si>
   <si>
     <t>Finite</t>
@@ -3080,7 +3080,7 @@
     <t>Stochastic</t>
   </si>
   <si>
-    <t>adpative dynamics</t>
+    <t>Adaptive Dynamics</t>
   </si>
   <si>
     <t>Analytical Model</t>

</xml_diff>